<commit_message>
use a simpler test case
</commit_message>
<xml_diff>
--- a/tests/testthat/sample_config/Test_validation.xlsx
+++ b/tests/testthat/sample_config/Test_validation.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Ethiopia-HEP-Capacity-Analysis\ehep\tests\bad_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Ethiopia-HEP-Capacity-Analysis\tests\testthat\sample_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A338F-8DC5-4FFC-9B12-404DC00542AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDEF81EE-ED7B-4D97-89FD-AB57749A01B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2960" windowWidth="29650" windowHeight="9250" activeTab="1" xr2:uid="{B3E9A58C-A710-4FBC-A24E-FA15ED7544EF}"/>
+    <workbookView xWindow="2340" yWindow="790" windowWidth="27240" windowHeight="13010" activeTab="2" xr2:uid="{B3E9A58C-A710-4FBC-A24E-FA15ED7544EF}"/>
   </bookViews>
   <sheets>
     <sheet name="SeasonalityCurves" sheetId="1" r:id="rId1"/>
     <sheet name="TaskValues_ref" sheetId="2" r:id="rId2"/>
-    <sheet name="Total_Pop2" sheetId="3" r:id="rId3"/>
+    <sheet name="StochasticParameters" sheetId="4" r:id="rId3"/>
+    <sheet name="Total_Pop2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2801" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="532">
   <si>
     <t>Month</t>
   </si>
@@ -1601,6 +1602,42 @@
   </si>
   <si>
     <t>FH.MN.ANC.1XX</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Fertility rates</t>
+  </si>
+  <si>
+    <t>Mortality rates</t>
+  </si>
+  <si>
+    <t>Incidence rates</t>
+  </si>
+  <si>
+    <t>Annual delta fertility rates</t>
+  </si>
+  <si>
+    <t>Annual delta mortality rates</t>
+  </si>
+  <si>
+    <t>Annual delta incidence rates</t>
+  </si>
+  <si>
+    <t>Seasonality ratio to mean</t>
+  </si>
+  <si>
+    <t>Minutes per contact</t>
+  </si>
+  <si>
+    <t>Hours per week</t>
   </si>
 </sst>
 </file>
@@ -2520,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7F5554-3BA4-46F6-B5C6-F7E042EE5330}">
   <dimension ref="A1:AA225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -16090,6 +16127,113 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316E6CA-92A7-4C84-96E1-892EBE8FB69D}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B5">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>527</v>
+      </c>
+      <c r="B6">
+        <v>0.22</v>
+      </c>
+      <c r="C6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>528</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>529</v>
+      </c>
+      <c r="B8">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>530</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>531</v>
+      </c>
+      <c r="B10">
+        <v>0.125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF05A38-A853-4925-B189-8985C9800629}">
   <dimension ref="A1:G102"/>
   <sheetViews>

</xml_diff>